<commit_message>
feat: complete starter kit with all 26 functions, 9 domains, VLM, pre-build validation
Starter Kit:
- Expanded from 5→9 domains (DM, AE, LB, CM, VS, DS, EX, MH, QS)
- Expanded from 44→115 variables covering all 26 derivation functions
- Expanded CT library: 13 codelists, ~48 terms
- VLM: 8 entries (3 LB.LBORRES + 5 VS.VSSTRESN)
- Added Method documentation sheet

Code:
- Implemented derive_visitdy() and derive_tpt() (were stubs)
- Added regex_extract/regex_replace/trim_pad switch cases
- Fixed coalesce/concat param name compatibility
- Fixed case_when to eval string-form conditions
- Fixed assign_ct identity pass-through (coded_value→coded_value)
- Added validate_prebuild() with 6 pre-build checks
- Integrated validate_prebuild() into check_end_to_end()

E2E: 9/9 domains PASS, 0 errors, 0 warnings
Tests: 264 PASS, 0 FAIL, 0 WARN
</commit_message>
<xml_diff>
--- a/inst/extdata/starter_kit/Study_CT.xlsx
+++ b/inst/extdata/starter_kit/Study_CT.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t xml:space="preserve">Select</t>
   </si>
@@ -187,6 +187,216 @@
   </si>
   <si>
     <t xml:space="preserve">Undifferentiated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VS Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C66741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSTESTCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VS Test Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C67153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSTEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No/Yes Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C66742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C66769</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AESEV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Route of Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C66729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disposition Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C66767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSCAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C71738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPOCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dose Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C71113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYSBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIABP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diastolic Blood Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODERATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEVERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTRAVENOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intravenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBCUTANEOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subcutaneous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROTOCOL MILESTONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protocol Milestone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPOSITION EVENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disposition Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCREENING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TREATMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOLLOW-UP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twice a Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Times a Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Four Times a Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every 2 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every 4 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every 6 Hours</t>
   </si>
 </sst>
 </file>
@@ -618,6 +828,142 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -948,6 +1294,530 @@
         <v>57</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44"/>
+      <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46"/>
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47"/>
+      <c r="E47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>